<commit_message>
new changes and some issues
</commit_message>
<xml_diff>
--- a/HRPortal .xlsx
+++ b/HRPortal .xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="61">
   <si>
     <t>SL No</t>
   </si>
@@ -181,6 +181,30 @@
   </si>
   <si>
     <t>Deducting TDS in payroll according to their Annual CTC</t>
+  </si>
+  <si>
+    <t>Bonus Column should add in payroll and should show in payslip if bonus present</t>
+  </si>
+  <si>
+    <t>Changes in PayrollDO, jsp and Util</t>
+  </si>
+  <si>
+    <t>Edit Access to HRUser also</t>
+  </si>
+  <si>
+    <t>Changes in viewemployee.jsp</t>
+  </si>
+  <si>
+    <t>Experience input field change to year and month</t>
+  </si>
+  <si>
+    <t>Changes in viewemployee.jsp &amp; addemployee.jsp</t>
+  </si>
+  <si>
+    <t>Update not working for middle name and languages known in employee</t>
+  </si>
+  <si>
+    <t>view employee  arrow images and showing same tab when again come to that page</t>
   </si>
 </sst>
 </file>
@@ -646,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1083,6 +1107,91 @@
         <v>50</v>
       </c>
     </row>
+    <row r="27" spans="1:5" ht="63">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="31.5">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="31.5">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="63">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="63">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>